<commit_message>
Completed overall data bucket pasting to all sheets
</commit_message>
<xml_diff>
--- a/Folder B/2022_5 Pluto.xlsx
+++ b/Folder B/2022_5 Pluto.xlsx
@@ -2,15 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="&lt;Worksheet &quot;Students by Core Subject&quot;&gt;" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Students Details" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Students Performance By Terms" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Students by Core Subject" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +51,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -167,7 +168,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -199,9 +200,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,6 +252,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,13 +450,1569 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A5:K43"/>
+  <dimension ref="A5:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Data Entry</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Class</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Contact</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Emergency Contact Name</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Relationship</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Zac</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Efron</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>123, ABC Road Street, America</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Kelly</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Aunt</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Abel</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Tesfaye</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>222, DDD Charlie Rd, America</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>222456098</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Abu</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Uncle</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Sam</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>223, DDD Charlie Rd Jr, America</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>123489208</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Jimmy</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Uncle</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Shahrukh</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Khan</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>5434, Xannie Rd, America</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>209390897</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Johnny</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Father</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Joe</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Jonas</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>5252 Jersey Rd, America</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>490274922</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Papa Jonas</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Father</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Nick</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Jonas</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>5252 Jersey Rd, America</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>458304203</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Papa Jonas</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Father</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Data Entry</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Class</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Emergency Contact Name</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Relationship</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Contact</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Contact Option</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Zac</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Efron</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Kelly</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Aunt</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Abel</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Tesfaye</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Abu</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Uncle</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Sam</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Jimmy</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Uncle</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>123489208</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Shahrukh</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Khan</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Johnny</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Father</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>209390897</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Joe</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Jonas</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Papa Jonas</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Father</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>490274922</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Nick</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Jonas</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Papa Jonas</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Father</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:H42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Data Entry</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Class</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Term</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Overall Performance</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>CGPA</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Class Rank</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Zac</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Efron</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Summer Exam 1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Abel</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Tesfaye</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Summer Exam 1</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Sam</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Summer Exam 1</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Shahrukh</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Khan</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Summer Exam 1</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Joe</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Jonas</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Summer Exam 1</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Nick</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Jonas</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Summer Exam 1</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Data Entry</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Class</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Term</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Overall Performance</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>CGPA</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Class Rank</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Zac</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Efron</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Winter Exam 1</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Abel</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Tesfaye</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Winter Exam 1</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H18" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Sam</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Winter Exam 1</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H19" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Shahrukh</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Khan</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Winter Exam 1</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Joe</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Jonas</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Winter Exam 1</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="H21" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Nick</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Jonas</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Winter Exam 1</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="H22" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Data Entry</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Class</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Term</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Overall Performance</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>CGPA</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Class Rank</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Zac</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Efron</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Pop Quiz Mathematics</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Abel</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Tesfaye</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Pop Quiz Mathematics</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Sam</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Pop Quiz Mathematics</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Shahrukh</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Khan</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Pop Quiz Mathematics</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Joe</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Jonas</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Pop Quiz Mathematics</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Nick</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Jonas</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Pop Quiz Mathematics</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Data Entry</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Class</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Term</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Overall Performance</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>CGPA</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Class Rank</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Zac</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Efron</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Final Exam</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>4</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Abel</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Tesfaye</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Final Exam</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>4</v>
+      </c>
+      <c r="H38" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Sam</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Final Exam</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>4</v>
+      </c>
+      <c r="H39" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Shahrukh</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Khan</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Final Exam</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>4</v>
+      </c>
+      <c r="H40" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Joe</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Jonas</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Final Exam</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>4</v>
+      </c>
+      <c r="H41" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Nick</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Jonas</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>5 Pluto</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Final Exam</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>4</v>
+      </c>
+      <c r="H42" t="n">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:K42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -495,17 +2088,17 @@
       <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Andrew</t>
+          <t>Zac</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Garfield</t>
+          <t>Efron</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -540,7 +2133,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -548,17 +2141,17 @@
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>Abel</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Holland</t>
+          <t>Tesfaye</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -568,12 +2161,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -588,12 +2181,12 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
           <t>B</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>A</t>
         </is>
       </c>
     </row>
@@ -601,17 +2194,17 @@
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Anthony</t>
+          <t>Sam</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Mackie</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -631,7 +2224,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -654,17 +2247,17 @@
       <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>Shahrukh</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Downey Jr</t>
+          <t>Khan</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -674,7 +2267,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -694,12 +2287,12 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -707,17 +2300,17 @@
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Chris</t>
+          <t>Joe</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Evans</t>
+          <t>Jonas</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -727,14 +2320,14 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>C</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
       <c r="H11" t="inlineStr">
         <is>
           <t>B</t>
@@ -747,7 +2340,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -760,17 +2353,17 @@
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Chris</t>
+          <t>Nick</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Hemsworth</t>
+          <t>Jonas</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -780,7 +2373,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -805,60 +2398,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Sebastian </t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Stan</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>5 Mercury</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Summer Exam 1</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>F</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -936,17 +2476,17 @@
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Andrew</t>
+          <t>Zac</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Garfield</t>
+          <t>Efron</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -989,17 +2529,17 @@
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>Abel</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Holland</t>
+          <t>Tesfaye</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1014,7 +2554,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1024,7 +2564,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1042,17 +2582,17 @@
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Anthony</t>
+          <t>Sam</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Mackie</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1072,17 +2612,17 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1095,17 +2635,17 @@
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>Shahrukh</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Downey Jr</t>
+          <t>Khan</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1115,7 +2655,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1148,17 +2688,17 @@
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Chris</t>
+          <t>Joe</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Evans</t>
+          <t>Jonas</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1178,7 +2718,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>B</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1193,7 +2733,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1201,17 +2741,17 @@
       <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Chris</t>
+          <t>Nick</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Hemsworth</t>
+          <t>Jonas</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1226,12 +2766,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>A</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1245,59 +2785,6 @@
         </is>
       </c>
       <c r="K22" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Sebastian </t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Stan</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>5 Mercury</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Winter Exam 1</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -1377,32 +2864,32 @@
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Andrew</t>
+          <t>Zac</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Garfield</t>
+          <t>Efron</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Pop Quiz (History)</t>
+          <t>Pop Quiz Mathematics</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
           <t>F</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1430,32 +2917,32 @@
       <c r="A28" t="inlineStr"/>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>Abel</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Holland</t>
+          <t>Tesfaye</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Pop Quiz (History)</t>
+          <t>Pop Quiz Mathematics</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
           <t>F</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1483,32 +2970,32 @@
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Anthony</t>
+          <t>Sam</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Mackie</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Pop Quiz (History)</t>
+          <t>Pop Quiz Mathematics</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
           <t>F</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1536,32 +3023,32 @@
       <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>Shahrukh</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Downey Jr</t>
+          <t>Khan</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Pop Quiz (History)</t>
+          <t>Pop Quiz Mathematics</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1589,32 +3076,32 @@
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Chris</t>
+          <t>Joe</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Evans</t>
+          <t>Jonas</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Pop Quiz (History)</t>
+          <t>Pop Quiz Mathematics</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1642,103 +3129,50 @@
       <c r="A32" t="inlineStr"/>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Chris</t>
+          <t>Nick</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Hemsworth</t>
+          <t>Jonas</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Pop Quiz (History)</t>
+          <t>Pop Quiz Mathematics</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
           <t>-</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
+      <c r="I32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
+      <c r="J32" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="K32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr"/>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Sebastian </t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Stan</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>5 Mercury</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Pop Quiz (History)</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1818,17 +3252,17 @@
       <c r="A37" t="inlineStr"/>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Andrew</t>
+          <t>Zac</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Garfield</t>
+          <t>Efron</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1871,17 +3305,17 @@
       <c r="A38" t="inlineStr"/>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>Abel</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Holland</t>
+          <t>Tesfaye</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1891,12 +3325,12 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -1916,7 +3350,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -1924,17 +3358,17 @@
       <c r="A39" t="inlineStr"/>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Anthony</t>
+          <t>Sam</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Mackie</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1944,7 +3378,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1969,7 +3403,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -1977,17 +3411,17 @@
       <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>Shahrukh</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Downey Jr</t>
+          <t>Khan</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1997,7 +3431,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -2030,17 +3464,17 @@
       <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Chris</t>
+          <t>Joe</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Evans</t>
+          <t>Jonas</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -2050,7 +3484,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -2070,12 +3504,12 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2083,17 +3517,17 @@
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Chris</t>
+          <t>Nick</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Hemsworth</t>
+          <t>Jonas</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>5 Mercury</t>
+          <t>5 Pluto</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -2103,7 +3537,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -2127,59 +3561,6 @@
         </is>
       </c>
       <c r="K42" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr"/>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Sebastian </t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Stan</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>5 Mercury</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Final Exam</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
         <is>
           <t>A</t>
         </is>

</xml_diff>